<commit_message>
Final - Add Huong Dan
</commit_message>
<xml_diff>
--- a/xnt/XNT_420014223.xlsx
+++ b/xnt/XNT_420014223.xlsx
@@ -2,15 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
-  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="202300"/>
+  <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\02_Code\02_VBA\18_Hana\Hana Code\hanaVBA\xnt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D47FCE13-8E98-4979-9F77-FE393CB511EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D6633AED-C1FC-40DF-A407-9875CCA0D607}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{BBAF782C-BE59-444C-862E-01046C2C7844}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{DAE7BCBB-AC48-4907-AE72-476336A6578B}"/>
   </bookViews>
   <sheets>
     <sheet name="xnt" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="184">
+  <si>
+    <t>Mã SP</t>
+  </si>
   <si>
     <t>Mã NL</t>
   </si>
@@ -56,51 +59,51 @@
     <t>120105326KD</t>
   </si>
   <si>
-    <t>105488736730</t>
+    <t>105488736730(5000)</t>
   </si>
   <si>
     <t>121003634KD</t>
   </si>
   <si>
-    <t>18-_x000D_
-105</t>
+    <t>18(2500)_x000D_
+105(22000)</t>
   </si>
   <si>
     <t>129901166KD</t>
   </si>
   <si>
-    <t>104717662340</t>
+    <t>104717662340(87500)</t>
   </si>
   <si>
     <t>129901239KD</t>
   </si>
   <si>
-    <t>105089995620</t>
+    <t>105089995620(648000)</t>
   </si>
   <si>
     <t>130400133KD</t>
   </si>
   <si>
-    <t>105172521640-_x000D_
-105</t>
+    <t>105172521640(1500)_x000D_
+105(35000)</t>
   </si>
   <si>
     <t>140100104KD</t>
   </si>
   <si>
-    <t>105048924410</t>
+    <t>105048924410(5000)</t>
   </si>
   <si>
     <t>140100108KD</t>
   </si>
   <si>
-    <t>105023106750</t>
+    <t>105023106750(5000)</t>
   </si>
   <si>
     <t>140100137KD</t>
   </si>
   <si>
-    <t>105152110600</t>
+    <t>105152110600(5000)</t>
   </si>
   <si>
     <t>140100206KD</t>
@@ -109,429 +112,534 @@
     <t>140100312KD</t>
   </si>
   <si>
-    <t>104413848010</t>
+    <t>104413848010(60000)</t>
   </si>
   <si>
     <t>140200000KD</t>
   </si>
   <si>
-    <t>104413846720</t>
+    <t>104413846720(528000)</t>
   </si>
   <si>
     <t>140200189KD</t>
   </si>
   <si>
-    <t>104708945460</t>
+    <t>104708945460(36000)</t>
   </si>
   <si>
     <t>140200207KD</t>
   </si>
   <si>
-    <t>105046733630-_x000D_
-105387762320</t>
+    <t>105046733630(2000)_x000D_
+105387762320(2000)</t>
   </si>
   <si>
     <t>140200586KD</t>
   </si>
   <si>
-    <t>104556725930</t>
+    <t>104556725930(4000)</t>
   </si>
   <si>
     <t>140200740KD</t>
   </si>
   <si>
-    <t>105152007330</t>
+    <t>105152007330(500)</t>
   </si>
   <si>
     <t>140300420KD</t>
   </si>
   <si>
-    <t>105152110600-_x000D_
-105</t>
+    <t>105152110600(3000)_x000D_
+105(132000)</t>
   </si>
   <si>
     <t>141100111KD</t>
   </si>
   <si>
+    <t>105152007330(1000)</t>
+  </si>
+  <si>
     <t>150100078KD</t>
   </si>
   <si>
-    <t>104612224400-_x000D_
-105042761500</t>
+    <t>104612224400(5000)_x000D_
+105042761500(5000)</t>
   </si>
   <si>
     <t>150101631KD</t>
   </si>
   <si>
-    <t>105042766950</t>
+    <t>105042766950(5000)</t>
   </si>
   <si>
     <t>150101750KD</t>
   </si>
   <si>
-    <t>105001578250</t>
+    <t>105001578250(5000)</t>
   </si>
   <si>
     <t>150101852KD</t>
   </si>
   <si>
-    <t>104395501560</t>
+    <t>104395501560(270000)</t>
   </si>
   <si>
     <t>150102446KD</t>
   </si>
   <si>
-    <t>104551965230-_x000D_
-105486136560</t>
+    <t>104551965230(5000)_x000D_
+105486136560(125000)</t>
   </si>
   <si>
     <t>150102789KD</t>
   </si>
   <si>
+    <t>105152110600(9338)</t>
+  </si>
+  <si>
     <t>150103334KD</t>
   </si>
   <si>
-    <t>105048949500-_x000D_
-105463210860</t>
+    <t>105048949500(10000)_x000D_
+105463210860(10000)</t>
   </si>
   <si>
     <t>150103825KD</t>
   </si>
   <si>
-    <t>104636904960-_x000D_
-105219026140-_x000D_
-105346181510</t>
+    <t>104636904960(10000)_x000D_
+105219026140(5000)_x000D_
+105346181510(5000)</t>
   </si>
   <si>
     <t>150104609KD</t>
   </si>
   <si>
-    <t>105408761140</t>
+    <t>105408761140(55000)</t>
   </si>
   <si>
     <t>150104806KD</t>
   </si>
   <si>
-    <t>105</t>
+    <t>105(5000)</t>
   </si>
   <si>
     <t>150201747KD</t>
   </si>
   <si>
-    <t>105042780400</t>
+    <t>105042780400(4000)</t>
   </si>
   <si>
     <t>150202517KD</t>
   </si>
   <si>
-    <t>18-_x000D_
-91</t>
+    <t>18(2000)_x000D_
+91(160000)</t>
   </si>
   <si>
     <t>150203066KD</t>
   </si>
   <si>
-    <t>105463210860</t>
+    <t>105463210860(10000)</t>
   </si>
   <si>
     <t>150203228KD</t>
   </si>
   <si>
-    <t>104637429040</t>
+    <t>104637429040(8000)</t>
   </si>
   <si>
     <t>150203229KD</t>
   </si>
   <si>
-    <t>104612230810</t>
+    <t>104612230810(4000)</t>
   </si>
   <si>
     <t>150203237KD</t>
   </si>
   <si>
-    <t>105273217120</t>
+    <t>105273217120(4000)</t>
   </si>
   <si>
     <t>150300080KD</t>
   </si>
   <si>
-    <t>105152110600-_x000D_
-122-_x000D_
-122</t>
+    <t>105152110600(3000)_x000D_
+122(2600)_x000D_
+122(12000)</t>
   </si>
   <si>
     <t>150300882KD</t>
   </si>
   <si>
-    <t>104413848340</t>
+    <t>104413848340(3000)</t>
   </si>
   <si>
     <t>150700765KD</t>
   </si>
   <si>
+    <t>105152110600(4000)_x000D_
+105(52000)</t>
+  </si>
+  <si>
     <t>151500138KD</t>
   </si>
   <si>
+    <t>105152110600(4000)</t>
+  </si>
+  <si>
     <t>151602832KD</t>
   </si>
   <si>
-    <t>105152007330-_x000D_
-122-_x000D_
-122</t>
+    <t>105152007330(1000)_x000D_
+122(1165)_x000D_
+122(2920)</t>
   </si>
   <si>
     <t>151603642KD</t>
   </si>
   <si>
-    <t>105152007330-_x000D_
-105</t>
+    <t>105152007330(1000)_x000D_
+105(2000)</t>
   </si>
   <si>
     <t>151603818KD</t>
   </si>
   <si>
+    <t>105152007330(1000)_x000D_
+105(3000)</t>
+  </si>
+  <si>
     <t>151604586KD</t>
   </si>
   <si>
-    <t>105184014830-_x000D_
-122</t>
+    <t>105184014830(100)_x000D_
+122(1532)</t>
   </si>
   <si>
     <t>15195035CKD</t>
   </si>
   <si>
-    <t>105184014830-_x000D_
-105</t>
+    <t>105184014830(97)_x000D_
+105(8689)</t>
   </si>
   <si>
     <t>152300278KD</t>
   </si>
   <si>
-    <t>401</t>
+    <t>401(3000)</t>
   </si>
   <si>
     <t>159900010KD</t>
   </si>
   <si>
-    <t>198</t>
+    <t>198(300000)</t>
   </si>
   <si>
     <t>159900011KD</t>
   </si>
   <si>
+    <t>198(42000)</t>
+  </si>
+  <si>
     <t>16160544BKD</t>
   </si>
   <si>
-    <t>105152007330-_x000D_
-122</t>
+    <t>105152007330(100)_x000D_
+122(297)</t>
   </si>
   <si>
     <t>16160573DKD</t>
   </si>
   <si>
-    <t>105167291500</t>
+    <t>105167291500(800)</t>
   </si>
   <si>
     <t>162302300KD</t>
   </si>
   <si>
-    <t>201-_x000D_
-519</t>
+    <t>201(16)_x000D_
+519(50)</t>
   </si>
   <si>
     <t>162302329KD</t>
   </si>
   <si>
-    <t>194-_x000D_
-7736</t>
+    <t>194(3)_x000D_
+7736(550)</t>
   </si>
   <si>
     <t>162302671KD</t>
   </si>
   <si>
-    <t>117-_x000D_
-89-_x000D_
-43128</t>
-  </si>
-  <si>
-    <t>104768442220</t>
-  </si>
-  <si>
-    <t>104873912730</t>
-  </si>
-  <si>
-    <t>105000449850-_x000D_
-105345618560-_x000D_
-105398668910</t>
-  </si>
-  <si>
-    <t>105102708430</t>
-  </si>
-  <si>
-    <t>104626353900-_x000D_
-104642726310</t>
-  </si>
-  <si>
-    <t>104626353900</t>
-  </si>
-  <si>
-    <t>104891827500</t>
-  </si>
-  <si>
-    <t>104917337600-_x000D_
-105108576640-_x000D_
-105144360310</t>
-  </si>
-  <si>
-    <t>104999387620</t>
-  </si>
-  <si>
-    <t>104907236820</t>
-  </si>
-  <si>
-    <t>105523932140-_x000D_
-105596083020</t>
-  </si>
-  <si>
-    <t>105398672520</t>
-  </si>
-  <si>
-    <t>105488791440</t>
-  </si>
-  <si>
-    <t>105439947540</t>
-  </si>
-  <si>
-    <t>105509475300</t>
-  </si>
-  <si>
-    <t>104621913540</t>
-  </si>
-  <si>
-    <t>105379313100</t>
-  </si>
-  <si>
-    <t>105083622560</t>
-  </si>
-  <si>
-    <t>104846747240</t>
-  </si>
-  <si>
-    <t>104626403450-_x000D_
-104658032510-_x000D_
-104674594030</t>
-  </si>
-  <si>
-    <t>104626403450</t>
-  </si>
-  <si>
-    <t>104626403450-_x000D_
-104658032510</t>
-  </si>
-  <si>
-    <t>105197767510</t>
-  </si>
-  <si>
-    <t>105506010260</t>
-  </si>
-  <si>
-    <t>104674594030</t>
-  </si>
-  <si>
-    <t>105273014600-_x000D_
-105398431460</t>
-  </si>
-  <si>
-    <t>105523932140</t>
-  </si>
-  <si>
-    <t>105273014600</t>
-  </si>
-  <si>
-    <t>104642726310</t>
-  </si>
-  <si>
-    <t>105462708300</t>
-  </si>
-  <si>
-    <t>104626403450-_x000D_
-105083663050</t>
-  </si>
-  <si>
-    <t>104905557740</t>
-  </si>
-  <si>
-    <t>105398686300</t>
-  </si>
-  <si>
-    <t>104626404630</t>
-  </si>
-  <si>
-    <t>104622402140</t>
-  </si>
-  <si>
-    <t>104975435460</t>
-  </si>
-  <si>
-    <t>104674594400</t>
-  </si>
-  <si>
-    <t>104674594400-_x000D_
-104733411160-_x000D_
-105083663050</t>
-  </si>
-  <si>
-    <t>105310942810</t>
-  </si>
-  <si>
-    <t>104928309730</t>
-  </si>
-  <si>
-    <t>105564468220</t>
-  </si>
-  <si>
-    <t>105509475300-_x000D_
-105596083020</t>
-  </si>
-  <si>
-    <t>105415696260</t>
-  </si>
-  <si>
-    <t>104658161420-_x000D_
-104789265710-_x000D_
-104906203250-_x000D_
-104969595840-_x000D_
-105102692920-_x000D_
-105509475300</t>
-  </si>
-  <si>
-    <t>105398689650</t>
-  </si>
-  <si>
-    <t>105523932140-_x000D_
-105596091860</t>
-  </si>
-  <si>
-    <t>105398693630</t>
-  </si>
-  <si>
-    <t>105317148860</t>
-  </si>
-  <si>
-    <t>105083666660</t>
-  </si>
-  <si>
-    <t>105596091860</t>
+    <t>117(50)_x000D_
+89(16)_x000D_
+43128(300)</t>
+  </si>
+  <si>
+    <t>104768442220(160000)</t>
+  </si>
+  <si>
+    <t>104873912730(20000)</t>
+  </si>
+  <si>
+    <t>105000449850(5000)_x000D_
+105345618560(5000)_x000D_
+105398668910(5000)</t>
+  </si>
+  <si>
+    <t>105102708430(5000)</t>
+  </si>
+  <si>
+    <t>104626353900(10000)_x000D_
+104642726310(50000)</t>
+  </si>
+  <si>
+    <t>104626353900(10000)</t>
+  </si>
+  <si>
+    <t>104891827500(36000)</t>
+  </si>
+  <si>
+    <t>104917337600(4000)_x000D_
+105108576640(8000)_x000D_
+105144360310(16000)</t>
+  </si>
+  <si>
+    <t>104999387620(12000)</t>
+  </si>
+  <si>
+    <t>104907236820(36000)</t>
+  </si>
+  <si>
+    <t>105523932140(1500)_x000D_
+105596083020(10500)</t>
+  </si>
+  <si>
+    <t>105398672520(156000)</t>
+  </si>
+  <si>
+    <t>105488791440(35000)</t>
+  </si>
+  <si>
+    <t>105398672520(15000)</t>
+  </si>
+  <si>
+    <t>105439947540(30000)</t>
+  </si>
+  <si>
+    <t>105509475300(5000)</t>
+  </si>
+  <si>
+    <t>105523932140(1000)_x000D_
+105596083020(8970)</t>
+  </si>
+  <si>
+    <t>104621913540(50000)</t>
+  </si>
+  <si>
+    <t>105379313100(10000)</t>
+  </si>
+  <si>
+    <t>105083622560(35000)</t>
+  </si>
+  <si>
+    <t>104846747240(10000)</t>
+  </si>
+  <si>
+    <t>104626403450(10000)_x000D_
+104658032510(10000)_x000D_
+104674594030(220000)</t>
+  </si>
+  <si>
+    <t>104626403450(20000)</t>
+  </si>
+  <si>
+    <t>104626403450(10000)_x000D_
+104658032510(20000)</t>
+  </si>
+  <si>
+    <t>105509475300(10000)</t>
+  </si>
+  <si>
+    <t>105197767510(20000)</t>
+  </si>
+  <si>
+    <t>105506010260(10000)</t>
+  </si>
+  <si>
+    <t>104674594030(20000)</t>
+  </si>
+  <si>
+    <t>105273014600(10000)_x000D_
+105398431460(40000)</t>
+  </si>
+  <si>
+    <t>105523932140(10000)</t>
+  </si>
+  <si>
+    <t>105523932140(5000)</t>
+  </si>
+  <si>
+    <t>105509475300(12000)</t>
+  </si>
+  <si>
+    <t>105273014600(10000)</t>
+  </si>
+  <si>
+    <t>104642726310(10000)</t>
+  </si>
+  <si>
+    <t>105462708300(10000)</t>
+  </si>
+  <si>
+    <t>105509475300(14500)</t>
+  </si>
+  <si>
+    <t>105083622560(50000)</t>
+  </si>
+  <si>
+    <t>104626403450(5000)_x000D_
+105083663050(20000)</t>
+  </si>
+  <si>
+    <t>105439947540(5000)</t>
+  </si>
+  <si>
+    <t>104905557740(15000)</t>
+  </si>
+  <si>
+    <t>105398686300(20000)</t>
+  </si>
+  <si>
+    <t>105523932140(5000)_x000D_
+105596083020(29990)</t>
+  </si>
+  <si>
+    <t>105197767510(24000)</t>
+  </si>
+  <si>
+    <t>104626404630(12000)</t>
+  </si>
+  <si>
+    <t>105506010260(4000)</t>
+  </si>
+  <si>
+    <t>104622402140(12000)</t>
+  </si>
+  <si>
+    <t>104975435460(176000)</t>
+  </si>
+  <si>
+    <t>105523932140(1000)_x000D_
+105596083020(5000)</t>
+  </si>
+  <si>
+    <t>105523932140(4000)_x000D_
+105596083020(33646)</t>
+  </si>
+  <si>
+    <t>104674594400(8000)</t>
+  </si>
+  <si>
+    <t>104674594400(8000)_x000D_
+104733411160(4000)_x000D_
+105083663050(28000)</t>
+  </si>
+  <si>
+    <t>105310942810(4000)</t>
+  </si>
+  <si>
+    <t>104928309730(118000)</t>
+  </si>
+  <si>
+    <t>105564468220(3000)</t>
+  </si>
+  <si>
+    <t>105509475300(2006)_x000D_
+105596083020(5990)</t>
+  </si>
+  <si>
+    <t>105523932140(3000)</t>
+  </si>
+  <si>
+    <t>105415696260(12000)</t>
+  </si>
+  <si>
+    <t>104658161420(3000)_x000D_
+104789265710(3000)_x000D_
+104906203250(3000)_x000D_
+104969595840(3000)_x000D_
+105102692920(6000)_x000D_
+105509475300(6000)</t>
+  </si>
+  <si>
+    <t>105398689650(15000)</t>
+  </si>
+  <si>
+    <t>105523932140(2061)_x000D_
+105596091860(6000)</t>
+  </si>
+  <si>
+    <t>104621913540(27000)</t>
+  </si>
+  <si>
+    <t>105523932140(3000)_x000D_
+105596091860(9000)</t>
+  </si>
+  <si>
+    <t>105415696260(18000)</t>
+  </si>
+  <si>
+    <t>105398693630(14000)</t>
+  </si>
+  <si>
+    <t>105317148860(3000)</t>
+  </si>
+  <si>
+    <t>105398693630(15000)</t>
+  </si>
+  <si>
+    <t>105083666660(5993)</t>
+  </si>
+  <si>
+    <t>105523932140(1500)_x000D_
+105596091860(4500)</t>
+  </si>
+  <si>
+    <t>105415696260(9000)</t>
+  </si>
+  <si>
+    <t>105509475300(3000)</t>
+  </si>
+  <si>
+    <t>105523932140(685)</t>
+  </si>
+  <si>
+    <t>105596091860(5000)</t>
   </si>
   <si>
     <t>15195035C</t>
   </si>
   <si>
-    <t>105524034600-_x000D_
-105596091860</t>
+    <t>105523932140(580)</t>
+  </si>
+  <si>
+    <t>105415696260(10000)</t>
+  </si>
+  <si>
+    <t>105596091860(4000)</t>
+  </si>
+  <si>
+    <t>105524034600(700)_x000D_
+105596091860(5004)</t>
   </si>
   <si>
     <t>16160544B</t>
+  </si>
+  <si>
+    <t>105524034600(2000)_x000D_
+105596091860(4000)</t>
   </si>
 </sst>
 </file>
@@ -568,11 +676,24 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
       <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -600,19 +721,19 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="표준 2" xfId="1" xr:uid="{C1471768-CFE1-41A9-8D03-DF32310ECBB5}"/>
+    <cellStyle name="표준 2" xfId="1" xr:uid="{42AA6FB3-E3E2-44F5-B0B5-606DE4D8425B}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -943,7 +1064,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C6A3638-6834-4396-BADE-D08E086917A6}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCABB780-AF64-457D-A113-AF5EFBBA7576}">
   <sheetPr codeName="Sheet8"/>
   <dimension ref="A1:F134"/>
   <sheetViews>
@@ -962,32 +1083,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1">
-        <v>420013837</v>
+      <c r="A1" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="2"/>
+      <c r="A2" s="2">
+        <v>420014223</v>
+      </c>
       <c r="B2" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D2" s="2">
         <v>149.99999999999994</v>
@@ -1000,12 +1123,14 @@
       </c>
     </row>
     <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="2"/>
+      <c r="A3" s="2">
+        <v>420014223</v>
+      </c>
       <c r="B3" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D3" s="2">
         <v>2964</v>
@@ -1018,12 +1143,14 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
+      <c r="A4" s="2">
+        <v>420014223</v>
+      </c>
       <c r="B4" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D4" s="2">
         <v>2371.2000000000003</v>
@@ -1036,12 +1163,14 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
+      <c r="A5" s="2">
+        <v>420014223</v>
+      </c>
       <c r="B5" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D5" s="2">
         <v>7410</v>
@@ -1054,12 +1183,14 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
+      <c r="A6" s="2">
+        <v>420014223</v>
+      </c>
       <c r="B6" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D6" s="2">
         <v>17784</v>
@@ -1072,12 +1203,14 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="2"/>
+      <c r="A7" s="2">
+        <v>420014223</v>
+      </c>
       <c r="B7" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D7" s="2">
         <v>2964</v>
@@ -1090,12 +1223,14 @@
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
+      <c r="A8" s="2">
+        <v>420014223</v>
+      </c>
       <c r="B8" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D8" s="2">
         <v>2964</v>
@@ -1108,12 +1243,14 @@
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="2"/>
+      <c r="A9" s="2">
+        <v>420014223</v>
+      </c>
       <c r="B9" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D9" s="2">
         <v>20.000000000000014</v>
@@ -1126,12 +1263,14 @@
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="2"/>
+      <c r="A10" s="2">
+        <v>420014223</v>
+      </c>
       <c r="B10" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D10" s="2">
         <v>2964</v>
@@ -1144,12 +1283,14 @@
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="2"/>
+      <c r="A11" s="2">
+        <v>420014223</v>
+      </c>
       <c r="B11" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D11" s="2">
         <v>11856</v>
@@ -1162,12 +1303,14 @@
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="2"/>
+      <c r="A12" s="2">
+        <v>420014223</v>
+      </c>
       <c r="B12" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D12" s="2">
         <v>2464.0000000000014</v>
@@ -1180,12 +1323,14 @@
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="2"/>
+      <c r="A13" s="2">
+        <v>420014223</v>
+      </c>
       <c r="B13" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D13" s="2">
         <v>5220.0000000000109</v>
@@ -1198,12 +1343,14 @@
       </c>
     </row>
     <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="2"/>
+      <c r="A14" s="2">
+        <v>420014223</v>
+      </c>
       <c r="B14" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D14" s="2">
         <v>2964</v>
@@ -1216,12 +1363,14 @@
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="2"/>
+      <c r="A15" s="2">
+        <v>420014223</v>
+      </c>
       <c r="B15" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D15" s="2">
         <v>1000.0000000000007</v>
@@ -1234,12 +1383,14 @@
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="2"/>
+      <c r="A16" s="2">
+        <v>420014223</v>
+      </c>
       <c r="B16" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D16" s="2">
         <v>42.999999999999872</v>
@@ -1252,12 +1403,14 @@
       </c>
     </row>
     <row r="17" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="2"/>
+      <c r="A17" s="2">
+        <v>420014223</v>
+      </c>
       <c r="B17" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D17" s="2">
         <v>20776.429999999997</v>
@@ -1270,12 +1423,14 @@
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="2"/>
+      <c r="A18" s="2">
+        <v>420014223</v>
+      </c>
       <c r="B18" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="D18" s="2">
         <v>380.99999999999858</v>
@@ -1288,12 +1443,14 @@
       </c>
     </row>
     <row r="19" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="2"/>
+      <c r="A19" s="2">
+        <v>420014223</v>
+      </c>
       <c r="B19" s="2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D19" s="2">
         <v>5928</v>
@@ -1306,12 +1463,14 @@
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="2"/>
+      <c r="A20" s="2">
+        <v>420014223</v>
+      </c>
       <c r="B20" s="2" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="D20" s="2">
         <v>2964</v>
@@ -1324,12 +1483,14 @@
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="2"/>
+      <c r="A21" s="2">
+        <v>420014223</v>
+      </c>
       <c r="B21" s="2" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D21" s="2">
         <v>2160.9969999999989</v>
@@ -1342,12 +1503,14 @@
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="2"/>
+      <c r="A22" s="2">
+        <v>420014223</v>
+      </c>
       <c r="B22" s="2" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D22" s="2">
         <v>4999.9999999999882</v>
@@ -1364,10 +1527,10 @@
         <v>420014223</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="D23" s="2">
         <v>8892</v>
@@ -1384,10 +1547,10 @@
         <v>420014223</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="D24" s="2">
         <v>5928</v>
@@ -1404,10 +1567,10 @@
         <v>420014223</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="D25" s="2">
         <v>14820</v>
@@ -1424,10 +1587,10 @@
         <v>420014223</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="D26" s="2">
         <v>18924.000000000018</v>
@@ -1444,10 +1607,10 @@
         <v>420014223</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="D27" s="2">
         <v>11856</v>
@@ -1464,10 +1627,10 @@
         <v>420014223</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="D28" s="2">
         <v>2964</v>
@@ -1484,10 +1647,10 @@
         <v>420014223</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="D29" s="2">
         <v>1000.0000000000007</v>
@@ -1504,10 +1667,10 @@
         <v>420014223</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="D30" s="2">
         <v>2964</v>
@@ -1524,10 +1687,10 @@
         <v>420014223</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="D31" s="2">
         <v>8892</v>
@@ -1544,10 +1707,10 @@
         <v>420014223</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="D32" s="2">
         <v>2999.9999999999877</v>
@@ -1564,10 +1727,10 @@
         <v>420014223</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="D33" s="2">
         <v>1499.9999999999998</v>
@@ -1584,10 +1747,10 @@
         <v>420014223</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="D34" s="2">
         <v>3865.9999999999854</v>
@@ -1604,10 +1767,10 @@
         <v>420014223</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="D35" s="2">
         <v>5892.0000000000127</v>
@@ -1624,10 +1787,10 @@
         <v>420014223</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="D36" s="2">
         <v>2999.9999999999877</v>
@@ -1644,10 +1807,10 @@
         <v>420014223</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>35</v>
+        <v>76</v>
       </c>
       <c r="D37" s="2">
         <v>26725.999999999989</v>
@@ -1664,10 +1827,10 @@
         <v>420014223</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>20</v>
+        <v>78</v>
       </c>
       <c r="D38" s="2">
         <v>2964</v>
@@ -1684,10 +1847,10 @@
         <v>420014223</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="D39" s="2">
         <v>2279</v>
@@ -1704,10 +1867,10 @@
         <v>420014223</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="D40" s="2">
         <v>2964</v>
@@ -1724,10 +1887,10 @@
         <v>420014223</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="D41" s="2">
         <v>1429.9999999999995</v>
@@ -1744,10 +1907,10 @@
         <v>420014223</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="D42" s="2">
         <v>1531.9999999999993</v>
@@ -1764,10 +1927,10 @@
         <v>420014223</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="D43" s="2">
         <v>330.99999999999926</v>
@@ -1784,10 +1947,10 @@
         <v>420014223</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="D44" s="2">
         <v>2964</v>
@@ -1804,10 +1967,10 @@
         <v>420014223</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="D45" s="2">
         <v>4446</v>
@@ -1824,10 +1987,10 @@
         <v>420014223</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>86</v>
+        <v>94</v>
       </c>
       <c r="D46" s="2">
         <v>3302.000000000005</v>
@@ -1844,10 +2007,10 @@
         <v>420014223</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>88</v>
+        <v>95</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>89</v>
+        <v>96</v>
       </c>
       <c r="D47" s="2">
         <v>297.00000000000131</v>
@@ -1864,10 +2027,10 @@
         <v>420014223</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>90</v>
+        <v>97</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>91</v>
+        <v>98</v>
       </c>
       <c r="D48" s="2">
         <v>126.00000000000006</v>
@@ -1884,10 +2047,10 @@
         <v>420014223</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>92</v>
+        <v>99</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>93</v>
+        <v>100</v>
       </c>
       <c r="D49" s="2">
         <v>36.370999999999952</v>
@@ -1904,10 +2067,10 @@
         <v>420014223</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>94</v>
+        <v>101</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>95</v>
+        <v>102</v>
       </c>
       <c r="D50" s="2">
         <v>68.738000000000085</v>
@@ -1924,10 +2087,10 @@
         <v>420014223</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>97</v>
+        <v>104</v>
       </c>
       <c r="D51" s="2">
         <v>100.77600000000001</v>
@@ -1947,7 +2110,7 @@
         <v>140100100</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="D52" s="2">
         <v>5500.0000000000118</v>
@@ -1967,7 +2130,7 @@
         <v>140100102</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>99</v>
+        <v>106</v>
       </c>
       <c r="D53" s="2">
         <v>1895.3849999999989</v>
@@ -1987,7 +2150,7 @@
         <v>140100112</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>99</v>
+        <v>106</v>
       </c>
       <c r="D54" s="2">
         <v>10016.000000000011</v>
@@ -2007,7 +2170,7 @@
         <v>140100114</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>100</v>
+        <v>107</v>
       </c>
       <c r="D55" s="2">
         <v>11856</v>
@@ -2027,7 +2190,7 @@
         <v>140100199</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>101</v>
+        <v>108</v>
       </c>
       <c r="D56" s="2">
         <v>2964</v>
@@ -2047,7 +2210,7 @@
         <v>140100253</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>102</v>
+        <v>109</v>
       </c>
       <c r="D57" s="2">
         <v>17784</v>
@@ -2067,7 +2230,7 @@
         <v>140100490</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>103</v>
+        <v>110</v>
       </c>
       <c r="D58" s="2">
         <v>5928</v>
@@ -2087,7 +2250,7 @@
         <v>140200097</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>104</v>
+        <v>111</v>
       </c>
       <c r="D59" s="2">
         <v>4928.0000000000146</v>
@@ -2107,7 +2270,7 @@
         <v>140200189</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>105</v>
+        <v>112</v>
       </c>
       <c r="D60" s="2">
         <v>27383.999999999989</v>
@@ -2127,7 +2290,7 @@
         <v>140200190</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>106</v>
+        <v>113</v>
       </c>
       <c r="D61" s="2">
         <v>5928</v>
@@ -2147,7 +2310,7 @@
         <v>140200191</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>107</v>
+        <v>114</v>
       </c>
       <c r="D62" s="2">
         <v>2964</v>
@@ -2167,7 +2330,7 @@
         <v>140200740</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>108</v>
+        <v>115</v>
       </c>
       <c r="D63" s="2">
         <v>5884.9999999999982</v>
@@ -2187,7 +2350,7 @@
         <v>140300057</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>109</v>
+        <v>116</v>
       </c>
       <c r="D64" s="2">
         <v>29640</v>
@@ -2207,7 +2370,7 @@
         <v>140300469</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>110</v>
+        <v>117</v>
       </c>
       <c r="D65" s="2">
         <v>5928</v>
@@ -2227,7 +2390,7 @@
         <v>140300470</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>109</v>
+        <v>118</v>
       </c>
       <c r="D66" s="2">
         <v>2964</v>
@@ -2247,7 +2410,7 @@
         <v>140400029</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>111</v>
+        <v>119</v>
       </c>
       <c r="D67" s="2">
         <v>8910.951999999992</v>
@@ -2267,7 +2430,7 @@
         <v>140400094</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>112</v>
+        <v>120</v>
       </c>
       <c r="D68" s="2">
         <v>2988.9999999999936</v>
@@ -2287,7 +2450,7 @@
         <v>141100111</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>108</v>
+        <v>121</v>
       </c>
       <c r="D69" s="2">
         <v>2583.0000000000014</v>
@@ -2307,7 +2470,7 @@
         <v>150100029</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>113</v>
+        <v>122</v>
       </c>
       <c r="D70" s="2">
         <v>6321.1070000000118</v>
@@ -2327,7 +2490,7 @@
         <v>150100408</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>114</v>
+        <v>123</v>
       </c>
       <c r="D71" s="2">
         <v>40.000000000000028</v>
@@ -2347,7 +2510,7 @@
         <v>150101750</v>
       </c>
       <c r="C72" s="3" t="s">
-        <v>115</v>
+        <v>124</v>
       </c>
       <c r="D72" s="2">
         <v>803.00300000000107</v>
@@ -2367,7 +2530,7 @@
         <v>150101758</v>
       </c>
       <c r="C73" s="3" t="s">
-        <v>116</v>
+        <v>125</v>
       </c>
       <c r="D73" s="2">
         <v>1840.0000000000002</v>
@@ -2387,7 +2550,7 @@
         <v>150101849</v>
       </c>
       <c r="C74" s="3" t="s">
-        <v>117</v>
+        <v>126</v>
       </c>
       <c r="D74" s="2">
         <v>23712</v>
@@ -2407,7 +2570,7 @@
         <v>150101850</v>
       </c>
       <c r="C75" s="3" t="s">
-        <v>118</v>
+        <v>127</v>
       </c>
       <c r="D75" s="2">
         <v>17784</v>
@@ -2427,7 +2590,7 @@
         <v>150101852</v>
       </c>
       <c r="C76" s="3" t="s">
-        <v>119</v>
+        <v>128</v>
       </c>
       <c r="D76" s="2">
         <v>21676.000000000011</v>
@@ -2447,7 +2610,7 @@
         <v>150102390</v>
       </c>
       <c r="C77" s="3" t="s">
-        <v>112</v>
+        <v>129</v>
       </c>
       <c r="D77" s="2">
         <v>2964</v>
@@ -2467,7 +2630,7 @@
         <v>150102422</v>
       </c>
       <c r="C78" s="3" t="s">
-        <v>120</v>
+        <v>130</v>
       </c>
       <c r="D78" s="2">
         <v>17784</v>
@@ -2487,7 +2650,7 @@
         <v>150102456</v>
       </c>
       <c r="C79" s="3" t="s">
-        <v>121</v>
+        <v>131</v>
       </c>
       <c r="D79" s="2">
         <v>2992.4299999999957</v>
@@ -2507,7 +2670,7 @@
         <v>150102960</v>
       </c>
       <c r="C80" s="3" t="s">
-        <v>122</v>
+        <v>132</v>
       </c>
       <c r="D80" s="2">
         <v>2964</v>
@@ -2527,7 +2690,7 @@
         <v>150102978</v>
       </c>
       <c r="C81" s="3" t="s">
-        <v>123</v>
+        <v>133</v>
       </c>
       <c r="D81" s="2">
         <v>17784</v>
@@ -2547,7 +2710,7 @@
         <v>150103021</v>
       </c>
       <c r="C82" s="3" t="s">
-        <v>124</v>
+        <v>134</v>
       </c>
       <c r="D82" s="2">
         <v>5928</v>
@@ -2567,7 +2730,7 @@
         <v>150103142</v>
       </c>
       <c r="C83" s="3" t="s">
-        <v>124</v>
+        <v>135</v>
       </c>
       <c r="D83" s="2">
         <v>2813.9999999999991</v>
@@ -2587,7 +2750,7 @@
         <v>150103485</v>
       </c>
       <c r="C84" s="3" t="s">
-        <v>112</v>
+        <v>136</v>
       </c>
       <c r="D84" s="2">
         <v>2964</v>
@@ -2607,7 +2770,7 @@
         <v>150103654</v>
       </c>
       <c r="C85" s="3" t="s">
-        <v>112</v>
+        <v>120</v>
       </c>
       <c r="D85" s="2">
         <v>2964</v>
@@ -2627,7 +2790,7 @@
         <v>150103825</v>
       </c>
       <c r="C86" s="3" t="s">
-        <v>118</v>
+        <v>127</v>
       </c>
       <c r="D86" s="2">
         <v>8180.0000000000018</v>
@@ -2647,7 +2810,7 @@
         <v>150103965</v>
       </c>
       <c r="C87" s="3" t="s">
-        <v>125</v>
+        <v>137</v>
       </c>
       <c r="D87" s="2">
         <v>7205.1069999999881</v>
@@ -2667,7 +2830,7 @@
         <v>150104135</v>
       </c>
       <c r="C88" s="3" t="s">
-        <v>126</v>
+        <v>138</v>
       </c>
       <c r="D88" s="2">
         <v>8892</v>
@@ -2687,7 +2850,7 @@
         <v>150104191</v>
       </c>
       <c r="C89" s="3" t="s">
-        <v>127</v>
+        <v>139</v>
       </c>
       <c r="D89" s="2">
         <v>1686.8929999999993</v>
@@ -2707,7 +2870,7 @@
         <v>150104201</v>
       </c>
       <c r="C90" s="3" t="s">
-        <v>112</v>
+        <v>140</v>
       </c>
       <c r="D90" s="2">
         <v>11856</v>
@@ -2727,7 +2890,7 @@
         <v>150104270</v>
       </c>
       <c r="C91" s="3" t="s">
-        <v>112</v>
+        <v>120</v>
       </c>
       <c r="D91" s="2">
         <v>2964</v>
@@ -2747,7 +2910,7 @@
         <v>150104306</v>
       </c>
       <c r="C92" s="3" t="s">
-        <v>115</v>
+        <v>141</v>
       </c>
       <c r="D92" s="2">
         <v>2964</v>
@@ -2767,7 +2930,7 @@
         <v>150104318</v>
       </c>
       <c r="C93" s="3" t="s">
-        <v>128</v>
+        <v>142</v>
       </c>
       <c r="D93" s="2">
         <v>6996.6150000000043</v>
@@ -2787,7 +2950,7 @@
         <v>150104324</v>
       </c>
       <c r="C94" s="3" t="s">
-        <v>111</v>
+        <v>143</v>
       </c>
       <c r="D94" s="2">
         <v>2964</v>
@@ -2807,7 +2970,7 @@
         <v>150104386</v>
       </c>
       <c r="C95" s="3" t="s">
-        <v>129</v>
+        <v>144</v>
       </c>
       <c r="D95" s="2">
         <v>2570.8930000000005</v>
@@ -2827,7 +2990,7 @@
         <v>150104598</v>
       </c>
       <c r="C96" s="3" t="s">
-        <v>130</v>
+        <v>145</v>
       </c>
       <c r="D96" s="2">
         <v>8892</v>
@@ -2847,7 +3010,7 @@
         <v>150104839</v>
       </c>
       <c r="C97" s="3" t="s">
-        <v>108</v>
+        <v>146</v>
       </c>
       <c r="D97" s="2">
         <v>17784</v>
@@ -2867,7 +3030,7 @@
         <v>150200042</v>
       </c>
       <c r="C98" s="3" t="s">
-        <v>120</v>
+        <v>147</v>
       </c>
       <c r="D98" s="2">
         <v>28.430000000000014</v>
@@ -2887,7 +3050,7 @@
         <v>150200380</v>
       </c>
       <c r="C99" s="3" t="s">
-        <v>131</v>
+        <v>148</v>
       </c>
       <c r="D99" s="2">
         <v>499.99999999999886</v>
@@ -2907,7 +3070,7 @@
         <v>150201086</v>
       </c>
       <c r="C100" s="3" t="s">
-        <v>121</v>
+        <v>149</v>
       </c>
       <c r="D100" s="2">
         <v>2964</v>
@@ -2927,7 +3090,7 @@
         <v>150201205</v>
       </c>
       <c r="C101" s="3" t="s">
-        <v>132</v>
+        <v>150</v>
       </c>
       <c r="D101" s="2">
         <v>8892</v>
@@ -2947,7 +3110,7 @@
         <v>150201734</v>
       </c>
       <c r="C102" s="3" t="s">
-        <v>133</v>
+        <v>151</v>
       </c>
       <c r="D102" s="2">
         <v>4928.0000000000146</v>
@@ -2967,7 +3130,7 @@
         <v>150201999</v>
       </c>
       <c r="C103" s="3" t="s">
-        <v>108</v>
+        <v>152</v>
       </c>
       <c r="D103" s="2">
         <v>2964</v>
@@ -2987,7 +3150,7 @@
         <v>150203119</v>
       </c>
       <c r="C104" s="3" t="s">
-        <v>108</v>
+        <v>153</v>
       </c>
       <c r="D104" s="2">
         <v>17784</v>
@@ -3007,7 +3170,7 @@
         <v>150203227</v>
       </c>
       <c r="C105" s="3" t="s">
-        <v>134</v>
+        <v>154</v>
       </c>
       <c r="D105" s="2">
         <v>5928</v>
@@ -3027,7 +3190,7 @@
         <v>150203228</v>
       </c>
       <c r="C106" s="3" t="s">
-        <v>135</v>
+        <v>155</v>
       </c>
       <c r="D106" s="2">
         <v>17748.000000000015</v>
@@ -3047,7 +3210,7 @@
         <v>150203237</v>
       </c>
       <c r="C107" s="3" t="s">
-        <v>136</v>
+        <v>156</v>
       </c>
       <c r="D107" s="2">
         <v>3526.0000000000059</v>
@@ -3067,7 +3230,7 @@
         <v>150203267</v>
       </c>
       <c r="C108" s="3" t="s">
-        <v>137</v>
+        <v>157</v>
       </c>
       <c r="D108" s="2">
         <v>8892</v>
@@ -3087,7 +3250,7 @@
         <v>150300080</v>
       </c>
       <c r="C109" s="3" t="s">
-        <v>138</v>
+        <v>158</v>
       </c>
       <c r="D109" s="2">
         <v>2999.9999999999877</v>
@@ -3107,7 +3270,7 @@
         <v>150300423</v>
       </c>
       <c r="C110" s="3" t="s">
-        <v>139</v>
+        <v>159</v>
       </c>
       <c r="D110" s="2">
         <v>2964</v>
@@ -3127,7 +3290,7 @@
         <v>150300749</v>
       </c>
       <c r="C111" s="3" t="s">
-        <v>124</v>
+        <v>160</v>
       </c>
       <c r="D111" s="2">
         <v>2964</v>
@@ -3147,7 +3310,7 @@
         <v>150300826</v>
       </c>
       <c r="C112" s="3" t="s">
-        <v>140</v>
+        <v>161</v>
       </c>
       <c r="D112" s="2">
         <v>5928</v>
@@ -3167,7 +3330,7 @@
         <v>150300882</v>
       </c>
       <c r="C113" s="3" t="s">
-        <v>141</v>
+        <v>162</v>
       </c>
       <c r="D113" s="2">
         <v>23676.000000000015</v>
@@ -3187,7 +3350,7 @@
         <v>150301042</v>
       </c>
       <c r="C114" s="3" t="s">
-        <v>142</v>
+        <v>163</v>
       </c>
       <c r="D114" s="2">
         <v>2964</v>
@@ -3207,7 +3370,7 @@
         <v>150301786</v>
       </c>
       <c r="C115" s="3" t="s">
-        <v>143</v>
+        <v>164</v>
       </c>
       <c r="D115" s="2">
         <v>2988.9999999999936</v>
@@ -3227,7 +3390,7 @@
         <v>150400293</v>
       </c>
       <c r="C116" s="3" t="s">
-        <v>113</v>
+        <v>165</v>
       </c>
       <c r="D116" s="2">
         <v>5928</v>
@@ -3247,7 +3410,7 @@
         <v>150400464</v>
       </c>
       <c r="C117" s="3" t="s">
-        <v>143</v>
+        <v>166</v>
       </c>
       <c r="D117" s="2">
         <v>5928</v>
@@ -3267,7 +3430,7 @@
         <v>150400561</v>
       </c>
       <c r="C118" s="3" t="s">
-        <v>140</v>
+        <v>167</v>
       </c>
       <c r="D118" s="2">
         <v>5928</v>
@@ -3287,7 +3450,7 @@
         <v>150400746</v>
       </c>
       <c r="C119" s="3" t="s">
-        <v>144</v>
+        <v>168</v>
       </c>
       <c r="D119" s="2">
         <v>2982.9519999999925</v>
@@ -3307,7 +3470,7 @@
         <v>150401133</v>
       </c>
       <c r="C120" s="3" t="s">
-        <v>145</v>
+        <v>169</v>
       </c>
       <c r="D120" s="2">
         <v>2964</v>
@@ -3327,7 +3490,7 @@
         <v>151000171</v>
       </c>
       <c r="C121" s="3" t="s">
-        <v>144</v>
+        <v>170</v>
       </c>
       <c r="D121" s="2">
         <v>2988.9999999999936</v>
@@ -3347,7 +3510,7 @@
         <v>151000432</v>
       </c>
       <c r="C122" s="3" t="s">
-        <v>146</v>
+        <v>171</v>
       </c>
       <c r="D122" s="2">
         <v>2964</v>
@@ -3367,7 +3530,7 @@
         <v>151001659</v>
       </c>
       <c r="C123" s="3" t="s">
-        <v>143</v>
+        <v>172</v>
       </c>
       <c r="D123" s="2">
         <v>2992.7979999999975</v>
@@ -3387,7 +3550,7 @@
         <v>151002541</v>
       </c>
       <c r="C124" s="3" t="s">
-        <v>140</v>
+        <v>173</v>
       </c>
       <c r="D124" s="2">
         <v>2988.9999999999936</v>
@@ -3407,7 +3570,7 @@
         <v>151100548</v>
       </c>
       <c r="C125" s="3" t="s">
-        <v>112</v>
+        <v>174</v>
       </c>
       <c r="D125" s="2">
         <v>2964</v>
@@ -3427,7 +3590,7 @@
         <v>151600041</v>
       </c>
       <c r="C126" s="3" t="s">
-        <v>124</v>
+        <v>160</v>
       </c>
       <c r="D126" s="2">
         <v>2964</v>
@@ -3447,7 +3610,7 @@
         <v>151602832</v>
       </c>
       <c r="C127" s="3" t="s">
-        <v>124</v>
+        <v>175</v>
       </c>
       <c r="D127" s="2">
         <v>684.99999999999977</v>
@@ -3467,7 +3630,7 @@
         <v>151603818</v>
       </c>
       <c r="C128" s="3" t="s">
-        <v>138</v>
+        <v>158</v>
       </c>
       <c r="D128" s="2">
         <v>1534.0000000000005</v>
@@ -3487,7 +3650,7 @@
         <v>151604586</v>
       </c>
       <c r="C129" s="3" t="s">
-        <v>147</v>
+        <v>176</v>
       </c>
       <c r="D129" s="2">
         <v>1432.0000000000007</v>
@@ -3504,10 +3667,10 @@
         <v>420014223</v>
       </c>
       <c r="B130" s="2" t="s">
-        <v>148</v>
+        <v>177</v>
       </c>
       <c r="C130" s="3" t="s">
-        <v>124</v>
+        <v>178</v>
       </c>
       <c r="D130" s="2">
         <v>573.99999999999864</v>
@@ -3527,7 +3690,7 @@
         <v>152400820</v>
       </c>
       <c r="C131" s="3" t="s">
-        <v>140</v>
+        <v>179</v>
       </c>
       <c r="D131" s="2">
         <v>2964</v>
@@ -3547,7 +3710,7 @@
         <v>160101067</v>
       </c>
       <c r="C132" s="3" t="s">
-        <v>147</v>
+        <v>180</v>
       </c>
       <c r="D132" s="2">
         <v>2964</v>
@@ -3567,7 +3730,7 @@
         <v>161000260</v>
       </c>
       <c r="C133" s="3" t="s">
-        <v>149</v>
+        <v>181</v>
       </c>
       <c r="D133" s="2">
         <v>3031.0700000000147</v>
@@ -3584,10 +3747,10 @@
         <v>420014223</v>
       </c>
       <c r="B134" s="2" t="s">
-        <v>150</v>
+        <v>182</v>
       </c>
       <c r="C134" s="3" t="s">
-        <v>149</v>
+        <v>183</v>
       </c>
       <c r="D134" s="2">
         <v>2666.9999999999986</v>

</xml_diff>